<commit_message>
Change-Id: I24b94364ca3d09a0eefd2867a91ba891cc6e82f2 Signed-off-by: Noxolo Mandisa Mkhungo <noxolomandisamkhungo@gmail.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/sample_data.xlsx
+++ b/src/main/resources/sample_data.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCS\Documents\workspace\ess_portal\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCS\git\ess_portal\ess_portal\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
     <sheet name="EmployeeSalary" sheetId="2" r:id="rId2"/>
     <sheet name="CompanyOrgStructure" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,13 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Emp_Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -41,6 +35,63 @@
   </si>
   <si>
     <t>BOD</t>
+  </si>
+  <si>
+    <t>Employee Number</t>
+  </si>
+  <si>
+    <t>Limbani Ejiroghene</t>
+  </si>
+  <si>
+    <t>Idowu</t>
+  </si>
+  <si>
+    <t>Idir Faraji</t>
+  </si>
+  <si>
+    <t>Kayode</t>
+  </si>
+  <si>
+    <t>Imamu Chinedu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adebayo</t>
+  </si>
+  <si>
+    <t>Seti Siddhartha</t>
+  </si>
+  <si>
+    <t>Temitope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antigonos Rúni </t>
+  </si>
+  <si>
+    <t>Ayodele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kweku Julius </t>
+  </si>
+  <si>
+    <t>Arendse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raganhar Theoderich </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diodoros Cosmas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emmerich Ekkebert </t>
+  </si>
+  <si>
+    <t>Adebayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berhanu Arnviðr </t>
+  </si>
+  <si>
+    <t>Abiodun</t>
   </si>
 </sst>
 </file>
@@ -76,8 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,58 +410,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10011</v>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>18792</v>
+      </c>
+      <c r="D2">
+        <v>562261</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>10012</v>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>22980</v>
+      </c>
+      <c r="D3">
+        <v>800597</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10013</v>
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>23930</v>
+      </c>
+      <c r="D4">
+        <v>504991</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>10014</v>
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>24266</v>
+      </c>
+      <c r="D5">
+        <v>616129</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>10015</v>
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
+        <v>24323</v>
+      </c>
+      <c r="D6">
+        <v>660287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1">
+        <v>31038</v>
+      </c>
+      <c r="D7">
+        <v>943410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>31949</v>
+      </c>
+      <c r="D8">
+        <v>335292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
+        <v>34258</v>
+      </c>
+      <c r="D9">
+        <v>749890</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1">
+        <v>34580</v>
+      </c>
+      <c r="D10">
+        <v>625126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1">
+        <v>35373</v>
+      </c>
+      <c r="D11">
+        <v>908645</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D11">
+    <sortCondition ref="C11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -417,16 +590,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>